<commit_message>
vendor master ,vendor profile validation
work on country by state all done
</commit_message>
<xml_diff>
--- a/webroot/templates/line_master_upload.xlsx
+++ b/webroot/templates/line_master_upload.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\bsms\webroot\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC32A61-3199-4FFA-AB8C-44F72A734316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{30C76DB6-EE17-D84D-ABB1-A1A04F095F89}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>UOM</t>
   </si>
@@ -39,9 +38,6 @@
     <t>Line 1</t>
   </si>
   <si>
-    <t>NOS</t>
-  </si>
-  <si>
     <t>Line 2</t>
   </si>
   <si>
@@ -49,12 +45,24 @@
   </si>
   <si>
     <t>FACTORY_CODE</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>IND_TNA_Unit_1</t>
+  </si>
+  <si>
+    <t>IN_MA_TH_Unit1</t>
+  </si>
+  <si>
+    <t>__DA_Unit2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -399,11 +407,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0525033E-F9E9-E842-9FEF-26A9F0784B38}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -416,7 +424,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -429,33 +437,42 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
       <c r="C2">
         <v>1000</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
       <c r="C3">
         <v>5000</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
       <c r="C4">
         <v>500</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>